<commit_message>
project: filemanager read csv settings
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -1767,6 +1767,11 @@
           <t>3610899</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1784,6 +1789,11 @@
           <t>3610890</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1801,6 +1811,11 @@
           <t>3610887</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1818,6 +1833,11 @@
           <t>3610885</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1835,6 +1855,11 @@
           <t>3610879</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1852,6 +1877,11 @@
           <t>3610872</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1869,6 +1899,11 @@
           <t>3610817</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1886,6 +1921,11 @@
           <t>3610795</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1903,6 +1943,11 @@
           <t>3610773</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1920,6 +1965,11 @@
           <t>3610771</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1937,6 +1987,11 @@
           <t>3610770</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1954,6 +2009,11 @@
           <t>3610754</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1971,6 +2031,11 @@
           <t>3610752</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1988,6 +2053,11 @@
           <t>3610750</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2005,6 +2075,11 @@
           <t>3610748</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2022,6 +2097,11 @@
           <t>3610744</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2039,6 +2119,11 @@
           <t>3610740</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2056,6 +2141,11 @@
           <t>3610737</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2073,6 +2163,11 @@
           <t>3610734</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2090,6 +2185,11 @@
           <t>3610728</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3077,7 +3177,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3099,7 +3199,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3121,7 +3221,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3143,7 +3243,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3265,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3187,7 +3287,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3209,7 +3309,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3331,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -3253,7 +3353,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Ludmyla Stupnytska</t>
         </is>
       </c>
     </row>
@@ -9978,7 +10078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9992,8 +10092,6 @@
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="19.2" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -10012,11 +10110,6 @@
           <t>Lesia Korbutyak</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Maryna Mostishko</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -10049,16 +10142,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>GRANNL1531517</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -10091,16 +10174,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>GRANES36580</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10133,16 +10206,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>GRANSE116241</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10175,16 +10238,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>LP53525</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10217,16 +10270,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>GRANNL1531481</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10259,16 +10302,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>GRANNL1531479</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10301,16 +10334,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>GRANNL1531470</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10343,16 +10366,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>GRANDE155189</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10385,16 +10398,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>GRANNL1531446</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10427,16 +10430,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>VDNL19684</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10469,16 +10462,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>LP53522</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -10511,16 +10494,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>GRANNL1531422</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -10553,16 +10526,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>GRANSE116234</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -10595,16 +10558,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>GRANNL1531419</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -10637,16 +10590,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>GRANNL1531417</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -10679,16 +10622,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>GRANNL1531414</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -10721,16 +10654,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>GRANSE116232</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -10763,16 +10686,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>GRANNL1531400</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -10805,16 +10718,6 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>MYXL600920</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -10847,23 +10750,120 @@
           <t>2020-09-30</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>GRANNL1531390</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>GRANNL1531234</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>GRANNL1531229</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GRANNL1531223</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>GRANNL1531222</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>GRANNL1531220</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>GRANNL1531217</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>GRANNL1531216</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>GRANNL1531214</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2020-09-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>GRANNL1531212</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>2020-09-30</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>